<commit_message>
Data updates for 9 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35840C85-8C21-49A9-AC47-2D2DAE4FE56C}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC9C121D-8907-484D-9FD7-D219CA4480BB}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="490" windowWidth="25770" windowHeight="17090" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="22950" yWindow="-19125" windowWidth="17430" windowHeight="17085" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E101" si="3">1/D67</f>
+        <f t="shared" ref="E67:E102" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D101" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D102" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2420,6 +2420,25 @@
       <c r="E101" s="7">
         <f t="shared" si="3"/>
         <v>53.404265873015866</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" s="5">
+        <v>43930</v>
+      </c>
+      <c r="B102">
+        <v>113296</v>
+      </c>
+      <c r="C102">
+        <v>2349</v>
+      </c>
+      <c r="D102" s="2">
+        <f t="shared" si="4"/>
+        <v>2.0733300381302076E-2</v>
+      </c>
+      <c r="E102" s="7">
+        <f t="shared" si="3"/>
+        <v>48.231587909748825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for 10 Apr
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC9C121D-8907-484D-9FD7-D219CA4480BB}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1259EF3C-1E75-421D-A6D4-E562A9AB480D}"/>
   <bookViews>
-    <workbookView xWindow="22950" yWindow="-19125" windowWidth="17430" windowHeight="17085" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="22185" yWindow="-16905" windowWidth="16455" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E102" si="3">1/D67</f>
+        <f t="shared" ref="E67:E103" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D102" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D103" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2439,6 +2439,25 @@
       <c r="E102" s="7">
         <f t="shared" si="3"/>
         <v>48.231587909748825</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" s="5">
+        <v>43931</v>
+      </c>
+      <c r="B103">
+        <v>118235</v>
+      </c>
+      <c r="C103">
+        <v>2607</v>
+      </c>
+      <c r="D103" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2049308580369603E-2</v>
+      </c>
+      <c r="E103" s="7">
+        <f t="shared" si="3"/>
+        <v>45.352896049098582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for 12 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{04603C45-9D59-4889-B5BD-9651DE5A7CB6}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DC0459B6-AD12-411B-81F1-00E2B113D0AB}"/>
   <bookViews>
-    <workbookView xWindow="16410" yWindow="-20895" windowWidth="16455" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="20520" yWindow="-20385" windowWidth="16455" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E104" si="3">1/D67</f>
+        <f t="shared" ref="E67:E105" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D104" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D105" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2477,6 +2477,25 @@
       <c r="E104" s="7">
         <f t="shared" si="3"/>
         <v>44.653143274853804</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" s="5">
+        <v>43933</v>
+      </c>
+      <c r="B105">
+        <v>125452</v>
+      </c>
+      <c r="C105">
+        <v>2871</v>
+      </c>
+      <c r="D105" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2885246947039504E-2</v>
+      </c>
+      <c r="E105" s="7">
+        <f t="shared" si="3"/>
+        <v>43.69627307558342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for 14 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{15604E01-49A3-45EB-BD8A-3721FA634581}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B988B41-C387-44F3-B1CD-A803808685C2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E106" si="3">1/D67</f>
+        <f t="shared" ref="E67:E107" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D106" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D107" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2515,6 +2515,25 @@
       <c r="E106" s="7">
         <f t="shared" si="3"/>
         <v>42.307743216412973</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" s="5">
+        <v>43935</v>
+      </c>
+      <c r="B107">
+        <v>130072</v>
+      </c>
+      <c r="C107">
+        <v>3194</v>
+      </c>
+      <c r="D107" s="2">
+        <f t="shared" si="4"/>
+        <v>2.4555630727597023E-2</v>
+      </c>
+      <c r="E107" s="7">
+        <f t="shared" si="3"/>
+        <v>40.723857232310586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for 15 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B988B41-C387-44F3-B1CD-A803808685C2}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8045D262-2BE0-428A-B3FD-5EEBC56406ED}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="19560" yWindow="-19305" windowWidth="20520" windowHeight="17340" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+      <selection activeCell="L109" sqref="L109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E107" si="3">1/D67</f>
+        <f t="shared" ref="E67:E108" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D107" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D108" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2534,6 +2534,25 @@
       <c r="E107" s="7">
         <f t="shared" si="3"/>
         <v>40.723857232310586</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" s="5">
+        <v>43936</v>
+      </c>
+      <c r="B108">
+        <v>132210</v>
+      </c>
+      <c r="C108">
+        <v>3495</v>
+      </c>
+      <c r="D108" s="2">
+        <f t="shared" si="4"/>
+        <v>2.6435216700703427E-2</v>
+      </c>
+      <c r="E108" s="7">
+        <f t="shared" si="3"/>
+        <v>37.828326180257513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for 16 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8045D262-2BE0-428A-B3FD-5EEBC56406ED}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FCCC3298-382C-4013-B534-97E408F033C8}"/>
   <bookViews>
-    <workbookView xWindow="19560" yWindow="-19305" windowWidth="20520" windowHeight="17340" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="21735" yWindow="-20025" windowWidth="17895" windowHeight="18870" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="L109" sqref="L109"/>
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E108" si="3">1/D67</f>
+        <f t="shared" ref="E67:E109" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D108" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D109" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2553,6 +2553,25 @@
       <c r="E108" s="7">
         <f t="shared" si="3"/>
         <v>37.828326180257513</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="5">
+        <v>43937</v>
+      </c>
+      <c r="B109">
+        <v>134753</v>
+      </c>
+      <c r="C109">
+        <v>3804</v>
+      </c>
+      <c r="D109" s="2">
+        <f t="shared" si="4"/>
+        <v>2.8229427174163099E-2</v>
+      </c>
+      <c r="E109" s="7">
+        <f t="shared" si="3"/>
+        <v>35.424027339642478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for 21 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3118CFB-83D6-47E4-A05E-78804FEC5F76}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4169970F-F3F2-49D2-9B0D-8FF5059E39A9}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="560" windowWidth="25590" windowHeight="17080" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="21720" yWindow="-20340" windowWidth="17865" windowHeight="19425" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E113" si="3">1/D67</f>
+        <f t="shared" ref="E67:E114" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D113" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D114" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2648,6 +2648,25 @@
       <c r="E113" s="7">
         <f t="shared" si="3"/>
         <v>31.396596294700558</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" s="5">
+        <v>43942</v>
+      </c>
+      <c r="B114">
+        <v>147065</v>
+      </c>
+      <c r="C114">
+        <v>4862</v>
+      </c>
+      <c r="D114" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3060211471118213E-2</v>
+      </c>
+      <c r="E114" s="7">
+        <f t="shared" si="3"/>
+        <v>30.247840394899217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for 22 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4169970F-F3F2-49D2-9B0D-8FF5059E39A9}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3C47D09B-A087-4616-BC6A-B66FEA8400FA}"/>
   <bookViews>
-    <workbookView xWindow="21720" yWindow="-20340" windowWidth="17865" windowHeight="19425" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="15460" windowHeight="12950" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E114" si="3">1/D67</f>
+        <f t="shared" ref="E67:E115" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D114" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D115" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2667,6 +2667,25 @@
       <c r="E114" s="7">
         <f t="shared" si="3"/>
         <v>30.247840394899217</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" s="5">
+        <v>43943</v>
+      </c>
+      <c r="B115">
+        <v>148453</v>
+      </c>
+      <c r="C115">
+        <v>5086</v>
+      </c>
+      <c r="D115" s="2">
+        <f t="shared" si="4"/>
+        <v>3.4260001481950519E-2</v>
+      </c>
+      <c r="E115" s="7">
+        <f t="shared" si="3"/>
+        <v>29.188556822650412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for 23 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3C47D09B-A087-4616-BC6A-B66FEA8400FA}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2262D964-7165-488C-9A80-61F779450DB3}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="15460" windowHeight="12950" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="14865" yWindow="-20280" windowWidth="24345" windowHeight="19425" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+      <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E115" si="3">1/D67</f>
+        <f t="shared" ref="E67:E116" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D115" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D116" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2686,6 +2686,25 @@
       <c r="E115" s="7">
         <f t="shared" si="3"/>
         <v>29.188556822650412</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" s="5">
+        <v>43944</v>
+      </c>
+      <c r="B116">
+        <v>150729</v>
+      </c>
+      <c r="C116">
+        <v>5315</v>
+      </c>
+      <c r="D116" s="2">
+        <f t="shared" si="4"/>
+        <v>3.5261960206728629E-2</v>
+      </c>
+      <c r="E116" s="7">
+        <f t="shared" si="3"/>
+        <v>28.359172154280341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for 24 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2262D964-7165-488C-9A80-61F779450DB3}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{96F534F2-3267-4EAB-A90F-889298421A20}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="-20280" windowWidth="24345" windowHeight="19425" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
+    <workbookView xWindow="18300" yWindow="-20280" windowWidth="20910" windowHeight="19425" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="J119" sqref="J119"/>
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E116" si="3">1/D67</f>
+        <f t="shared" ref="E67:E117" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D116" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D117" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2705,6 +2705,25 @@
       <c r="E116" s="7">
         <f t="shared" si="3"/>
         <v>28.359172154280341</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="5">
+        <v>43945</v>
+      </c>
+      <c r="B117">
+        <v>153129</v>
+      </c>
+      <c r="C117">
+        <v>5575</v>
+      </c>
+      <c r="D117" s="2">
+        <f t="shared" si="4"/>
+        <v>3.6407212219762425E-2</v>
+      </c>
+      <c r="E117" s="7">
+        <f t="shared" si="3"/>
+        <v>27.467085201793719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for 26 April
</commit_message>
<xml_diff>
--- a/data/us/Case Estimate by German Rate.xlsx
+++ b/data/us/Case Estimate by German Rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{223D5481-00A1-4C18-A370-C4869AB8152B}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="114_{71F43BB6-729E-48F0-B937-F5A3F0B5E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{603703CD-A901-4653-8163-ECE24FBFD600}"/>
   <bookViews>
     <workbookView xWindow="970" yWindow="2080" windowWidth="24030" windowHeight="14330" firstSheet="1" activeTab="1" xr2:uid="{FFD06A75-49E6-446C-BE8B-0E6018D8909C}"/>
   </bookViews>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8F3BB6-7B1A-436F-81CB-5746A6DC9551}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="e">
-        <f t="shared" ref="E67:E118" si="3">1/D67</f>
+        <f t="shared" ref="E67:E119" si="3">1/D67</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>650</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93:D118" si="4">C93/B93</f>
+        <f t="shared" ref="D93:D119" si="4">C93/B93</f>
         <v>9.694113436041223E-3</v>
       </c>
       <c r="E93" s="7">
@@ -2743,6 +2743,25 @@
       <c r="E118" s="7">
         <f t="shared" si="3"/>
         <v>26.886422750130048</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="5">
+        <v>43947</v>
+      </c>
+      <c r="B119">
+        <v>156513</v>
+      </c>
+      <c r="C119">
+        <v>5877</v>
+      </c>
+      <c r="D119" s="2">
+        <f t="shared" si="4"/>
+        <v>3.7549596519138986E-2</v>
+      </c>
+      <c r="E119" s="7">
+        <f t="shared" si="3"/>
+        <v>26.631444614599285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>